<commit_message>
chat rest api works with memory, session-handling, context-aware. flutter frontend also works
</commit_message>
<xml_diff>
--- a/sysplan/requirements/requirements.xlsx
+++ b/sysplan/requirements/requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\munka\chat-app\chat\sysplan\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8206E69-A938-4563-9A5A-D28AE8C66C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15188795-A9FF-4F85-A671-2BA4C5993E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6E6044AC-418E-4FE1-A0AF-DD21874170A9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>Conversation/session control</t>
   </si>
@@ -131,51 +131,21 @@
     <t>User preference builder</t>
   </si>
   <si>
-    <t>After the first sign in, the users can give their favourite artists (max 10, min 0)</t>
-  </si>
-  <si>
-    <t>After the first sign in, the users can give their favourite galleries (max 10, min 0)</t>
-  </si>
-  <si>
-    <t>After the first sign in, the users can give their favourite artworks (max 10, min 0)</t>
-  </si>
-  <si>
     <t>The user preferences are stored in a db</t>
   </si>
   <si>
-    <t>After every visited gallery, the user preferences will be updated</t>
-  </si>
-  <si>
     <t>Multiple users can communicate with the AI at the same time</t>
   </si>
   <si>
-    <t>After 12 questions, the AI ends the conversation</t>
-  </si>
-  <si>
-    <t>In the end of the conversation, the AI asks whether the user wants to make an offer for the artwork, or not and continue the journey with a recommended artwork</t>
-  </si>
-  <si>
     <t>The previous messages are stored in db</t>
   </si>
   <si>
-    <t>World concepts/AI mapping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A few similar artworks can be recommended for each artwork by the recommendation engine </t>
-  </si>
-  <si>
     <t>Recommendation engine</t>
   </si>
   <si>
     <t>A recommendation is based on the last inspected artwork and the user preferences</t>
   </si>
   <si>
-    <t>In the db a few pregenerated questions are stored, which can be answered without sending a request to the AI</t>
-  </si>
-  <si>
-    <t>The users must indicate if they want to start a conversation</t>
-  </si>
-  <si>
     <t>In the beginning of the conversation the user can ask about the artwork or about the artist</t>
   </si>
   <si>
@@ -188,17 +158,297 @@
     <t>A user can be categorized as an impulsive or tematic customer, or an investor</t>
   </si>
   <si>
-    <t>Users who buy artworks in auctions have to be categorized as investors</t>
-  </si>
-  <si>
-    <t>Users who go to artfairs, cannot be categorized as investors</t>
+    <r>
+      <t xml:space="preserve">After </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> questions, the AI ends the conversation (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n = 12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>The users must indicate that they want to start a conversation</t>
+  </si>
+  <si>
+    <t>In the end of the conversation, the AI asks whether the user wants to make an offer for the artwork</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>If the user does not want to make an offer, continue with a recommended artwork</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the db </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> generated questions are being stored for every artwork, which can be answered without sending a request to the AI (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n = 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Data download</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> similar artworks can be recommended for each artwork by the recommendation engine (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n = 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>Users who go to art fairs, cannot be categorized as investors</t>
+  </si>
+  <si>
+    <t>Users who buy artworks in auctions are categorized as investors</t>
+  </si>
+  <si>
+    <t>Conversation generation</t>
+  </si>
+  <si>
+    <t>Prompt and completion both must be filtered by usage policy</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">After the first sign in, the users can select their favourite artists - min </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, max </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n = 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>m = 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>After the first sign in, the users can select their favourite galleries - min n, max m (n = 0, m = 10)</t>
+  </si>
+  <si>
+    <t>After the first sign in, the users can select their favourite artworks - min n, max m (n = 0, m = 10)</t>
+  </si>
+  <si>
+    <t>After every inspected artwork, the user preferences will be updated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,8 +481,17 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +501,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,9 +540,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -290,9 +552,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -607,287 +870,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAE0A97-33B6-4C29-BB03-2D533620EF7B}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="C22" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="C23" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="2" t="s">
+      <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-    </row>
     <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="A26" s="3"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>